<commit_message>
Se realizan los CP para cada HU, se ejecutan y documentan
</commit_message>
<xml_diff>
--- a/Pruebas_Manuales/Matriz_de_Trazabilidad.xlsx
+++ b/Pruebas_Manuales/Matriz_de_Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO\Desktop\Practicas-Personales\QA\Portafolio QA Automatizacion\Pruebas_Manuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FE544A-A403-451C-B4D9-32F0C5A9AB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292D2C6B-CA3F-47CE-9B98-41671940515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>ID Req</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Caso de Prueba</t>
   </si>
   <si>
-    <t>RF001</t>
-  </si>
-  <si>
     <t>El sistema debe permitir a los usuarios autenticarse con usuario y contraseña.</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>CP007</t>
   </si>
   <si>
-    <t>Validar que los campos obligatorios no estén vacíos.</t>
-  </si>
-  <si>
     <t>El sistema debe permitir editar información de empleados.</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>CP015</t>
   </si>
   <si>
-    <t>Validar que se puede aprobar o rechazar y que se notifica al empleado.</t>
-  </si>
-  <si>
     <t>El sistema debe permitir ver historial de solicitudes de vacaciones.</t>
   </si>
   <si>
@@ -238,13 +229,46 @@
   </si>
   <si>
     <t>RF013</t>
+  </si>
+  <si>
+    <t>Estado de prueba</t>
+  </si>
+  <si>
+    <t>RF001 - RF002</t>
+  </si>
+  <si>
+    <t>Pasado</t>
+  </si>
+  <si>
+    <t>Fallado</t>
+  </si>
+  <si>
+    <t>CP017</t>
+  </si>
+  <si>
+    <t>CP018</t>
+  </si>
+  <si>
+    <t>Validar mensaje de error para un id empleado ya existente</t>
+  </si>
+  <si>
+    <t>Validar comportamiento con campos vacios en el registro de empleados.</t>
+  </si>
+  <si>
+    <t>Validar que el nuevo empleado este en la lista de empleados del modulo PIM</t>
+  </si>
+  <si>
+    <t>Validar que se puede aprobar o rechazar solicitudes</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +300,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +317,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,6 +378,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,6 +684,7 @@
     <col min="5" max="5" width="19.109375" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="45" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.35">
@@ -634,7 +695,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -675,25 +736,31 @@
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H3" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
+      <c r="H4" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -702,10 +769,13 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>13</v>
+      <c r="H5" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -714,30 +784,36 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
+      <c r="H6" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>20</v>
+      <c r="H7" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -746,193 +822,260 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>22</v>
+      <c r="H8" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="F13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H13" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="H14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="F21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>65</v>
+      <c r="H21" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>